<commit_message>
Updated, another file for even runs
</commit_message>
<xml_diff>
--- a/data/elephant.xlsx
+++ b/data/elephant.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>x</t>
   </si>
@@ -20,6 +20,9 @@
   </si>
   <si>
     <t>Elephant</t>
+  </si>
+  <si>
+    <t>Another animal</t>
   </si>
 </sst>
 </file>
@@ -60,7 +63,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr/>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" rightToLeft="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100"/>
   </sheetViews>
@@ -76,16 +79,22 @@
       <c r="C1" s="0" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="0" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="2" spans="2:2">
       <c r="A2" s="0" t="n">
-        <v>-35</v>
+        <v>41</v>
       </c>
       <c r="B2" s="0" t="n">
-        <v>68</v>
+        <v>28</v>
       </c>
       <c r="C2" s="0" t="n">
-        <v>12</v>
+        <v>5</v>
+      </c>
+      <c r="D2" s="0" t="n">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update dependencies, license, readme
</commit_message>
<xml_diff>
--- a/data/elephant.xlsx
+++ b/data/elephant.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>x</t>
   </si>
@@ -20,9 +20,6 @@
   </si>
   <si>
     <t>Elephant</t>
-  </si>
-  <si>
-    <t>Another animal</t>
   </si>
 </sst>
 </file>
@@ -63,7 +60,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr/>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" rightToLeft="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100"/>
   </sheetViews>
@@ -79,22 +76,137 @@
       <c r="C1" s="0" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
-        <v>3</v>
-      </c>
     </row>
     <row r="2" spans="2:2">
       <c r="A2" s="0" t="n">
-        <v>41</v>
+        <v>-176</v>
       </c>
       <c r="B2" s="0" t="n">
-        <v>28</v>
+        <v>-156</v>
       </c>
       <c r="C2" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="3:3">
+      <c r="A3" s="0" t="n">
+        <v>-173</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>-158</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="4:4">
+      <c r="A4" s="0" t="n">
+        <v>-173</v>
+      </c>
+      <c r="B4" s="0" t="n">
+        <v>-77</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="5:5">
+      <c r="A5" s="0" t="n">
+        <v>-166</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <v>-46</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="6:6">
+      <c r="A6" s="0" t="n">
+        <v>-136</v>
+      </c>
+      <c r="B6" s="0" t="n">
+        <v>150</v>
+      </c>
+      <c r="C6" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="7:7">
+      <c r="A7" s="0" t="n">
+        <v>-126</v>
+      </c>
+      <c r="B7" s="0" t="n">
+        <v>-47</v>
+      </c>
+      <c r="C7" s="0" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="8:8">
+      <c r="A8" s="0" t="n">
+        <v>-126</v>
+      </c>
+      <c r="B8" s="0" t="n">
+        <v>73</v>
+      </c>
+      <c r="C8" s="0" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="9:9">
+      <c r="A9" s="0" t="n">
+        <v>-112</v>
+      </c>
+      <c r="B9" s="0" t="n">
+        <v>-115</v>
+      </c>
+      <c r="C9" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="D2" s="0" t="n">
-        <v>3</v>
+    </row>
+    <row r="10" spans="10:10">
+      <c r="A10" s="0" t="n">
+        <v>-102</v>
+      </c>
+      <c r="B10" s="0" t="n">
+        <v>-38</v>
+      </c>
+      <c r="C10" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="11:11">
+      <c r="A11" s="0" t="n">
+        <v>-61</v>
+      </c>
+      <c r="B11" s="0" t="n">
+        <v>-96</v>
+      </c>
+      <c r="C11" s="0" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="12:12">
+      <c r="A12" s="0" t="n">
+        <v>-53</v>
+      </c>
+      <c r="B12" s="0" t="n">
+        <v>-104</v>
+      </c>
+      <c r="C12" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="13:13">
+      <c r="A13" s="0" t="n">
+        <v>-48</v>
+      </c>
+      <c r="B13" s="0" t="n">
+        <v>-10</v>
+      </c>
+      <c r="C13" s="0" t="n">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>